<commit_message>
Added machine assignment handling
</commit_message>
<xml_diff>
--- a/test_files/Przykładowy szablon.xlsx
+++ b/test_files/Przykładowy szablon.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="12330"/>
@@ -12,14 +12,15 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$A$6:$R$6</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="109">
   <si>
     <t>Rodzaj</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Zakmet</t>
   </si>
   <si>
-    <t>Krawdziarka</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nazwa urządzenia: </t>
   </si>
   <si>
@@ -327,9 +325,6 @@
     <t>Koniec</t>
   </si>
   <si>
-    <t>Giętarka Jacek</t>
-  </si>
-  <si>
     <t>Wypalarka Sebastian</t>
   </si>
   <si>
@@ -349,6 +344,9 @@
   </si>
   <si>
     <t>S355</t>
+  </si>
+  <si>
+    <t>Gietarka Jacek</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1227,7 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1250,21 +1248,21 @@
       <c r="A1" s="10"/>
       <c r="B1" s="11"/>
       <c r="C1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="12"/>
       <c r="F1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="41"/>
       <c r="I1" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -1280,13 +1278,13 @@
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="42"/>
       <c r="I2" s="43"/>
@@ -1304,7 +1302,7 @@
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="17">
         <v>42566</v>
@@ -1312,13 +1310,13 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="20">
         <v>42496</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1334,7 +1332,7 @@
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="44">
         <f>H32</f>
@@ -1343,13 +1341,13 @@
       <c r="E4" s="44"/>
       <c r="F4" s="44"/>
       <c r="G4" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="23">
         <v>2</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1365,12 +1363,12 @@
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="46"/>
       <c r="E5" s="24"/>
       <c r="F5" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="22"/>
@@ -1417,10 +1415,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>11</v>
@@ -1429,33 +1427,33 @@
         <v>12</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="D7" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>59</v>
       </c>
       <c r="E7" s="28">
         <v>2</v>
@@ -1467,7 +1465,7 @@
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="8">
         <v>30</v>
@@ -1477,23 +1475,23 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="28">
         <v>2</v>
@@ -1501,17 +1499,17 @@
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
       <c r="H8" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="8">
         <v>30</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -1522,58 +1520,54 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="28">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="8">
         <v>30</v>
       </c>
       <c r="L9" s="8"/>
-      <c r="M9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="28">
         <v>1</v>
@@ -1581,101 +1575,97 @@
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="27" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="8">
         <v>30</v>
       </c>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="M10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="Q10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="E11" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="27" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K11" s="8">
-        <v>20</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>56</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
-      <c r="N11" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N11" s="8"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="E12" s="28">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="27" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K12" s="8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -1684,154 +1674,158 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>38</v>
-      </c>
       <c r="C13" s="27" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E13" s="28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="27" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="8">
         <v>20</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="P13" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E14" s="28">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" s="8">
         <v>20</v>
       </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E15" s="28">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" s="8">
         <v>20</v>
       </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="M15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="8"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="Q15" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="R15" s="8"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E16" s="28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
       <c r="H16" s="27" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K16" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
@@ -1840,78 +1834,78 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E17" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="27" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K17" s="8">
-        <v>10</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M17" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>52</v>
-      </c>
       <c r="C18" s="27" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E18" s="28">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
       <c r="H18" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" s="30"/>
       <c r="J18" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K18" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -1920,36 +1914,36 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E19" s="28">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="27" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="I19" s="30"/>
       <c r="J19" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K19" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
@@ -1958,36 +1952,36 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E20" s="28">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="27" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
       <c r="I20" s="30"/>
       <c r="J20" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K20" s="8">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
@@ -1996,113 +1990,117 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E21" s="28">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="27" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="I21" s="30"/>
       <c r="J21" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" s="8">
-        <v>20</v>
-      </c>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8" t="s">
-        <v>56</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="8"/>
       <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="O21" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
+      <c r="Q21" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E22" s="28">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="30"/>
       <c r="J22" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" s="8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E23" s="28">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="27" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="M23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
@@ -2110,76 +2108,74 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="E24" s="28">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="30"/>
       <c r="J24" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K24" s="8">
         <v>20</v>
       </c>
       <c r="L24" s="8"/>
-      <c r="M24" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="M24" s="8"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="O24" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="P24" s="8"/>
-      <c r="Q24" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1">
       <c r="A25" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="E25" s="28">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I25" s="30"/>
       <c r="J25" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K25" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
@@ -2193,7 +2189,7 @@
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
       <c r="F26" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="37">
         <f>SUM(G6:G25)</f>
@@ -2213,13 +2209,13 @@
     </row>
     <row r="30" spans="1:18">
       <c r="C30" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="39" t="s">
         <v>83</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2227,10 +2223,10 @@
         <v>10</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2241,7 +2237,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="3:5">
@@ -2252,104 +2248,109 @@
         <v>12</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="3:5">
       <c r="C34" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="39" t="s">
         <v>86</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="35" spans="3:5">
       <c r="C35" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="39" t="s">
         <v>99</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="3:5">
       <c r="C39" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="3:5">
       <c r="C40" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="39" t="s">
         <v>88</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="41" spans="3:5">
       <c r="C41" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="3:5">
       <c r="C42" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="3:5">
       <c r="C43" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="3:5">
       <c r="C44" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="3:5">
       <c r="C45" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="3:5">
       <c r="C46" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="3:5">
       <c r="C47" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A6:R6">
+    <sortState ref="A7:R26">
+      <sortCondition ref="C6"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="5">
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G2:I2"/>

</xml_diff>

<commit_message>
Added static method defineTechnology() and static variables: cut2DList, benderList.
</commit_message>
<xml_diff>
--- a/test_files/Przykładowy szablon.xlsx
+++ b/test_files/Przykładowy szablon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
   <si>
     <t>Rodzaj</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Zakmet</t>
   </si>
   <si>
-    <t>Krawdziarka</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nazwa urządzenia: </t>
   </si>
   <si>
@@ -327,9 +324,6 @@
     <t>Koniec</t>
   </si>
   <si>
-    <t>Giętarka Jacek</t>
-  </si>
-  <si>
     <t>Wypalarka Sebastian</t>
   </si>
   <si>
@@ -349,6 +343,9 @@
   </si>
   <si>
     <t>S355</t>
+  </si>
+  <si>
+    <t>Gietarka Jacek</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1226,7 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1250,21 +1247,21 @@
       <c r="A1" s="10"/>
       <c r="B1" s="11"/>
       <c r="C1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="12"/>
       <c r="F1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="41"/>
       <c r="I1" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -1280,13 +1277,13 @@
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="42"/>
       <c r="I2" s="43"/>
@@ -1304,7 +1301,7 @@
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="17">
         <v>42566</v>
@@ -1312,13 +1309,13 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="20">
         <v>42496</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
@@ -1334,7 +1331,7 @@
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="44">
         <f>H32</f>
@@ -1343,13 +1340,13 @@
       <c r="E4" s="44"/>
       <c r="F4" s="44"/>
       <c r="G4" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="23">
         <v>2</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1365,12 +1362,12 @@
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="46"/>
       <c r="E5" s="24"/>
       <c r="F5" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="48"/>
       <c r="H5" s="22"/>
@@ -1417,10 +1414,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>11</v>
@@ -1429,33 +1426,33 @@
         <v>12</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="D7" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>59</v>
       </c>
       <c r="E7" s="28">
         <v>2</v>
@@ -1467,7 +1464,7 @@
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="8">
         <v>30</v>
@@ -1477,23 +1474,23 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
       <c r="P7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="28">
         <v>2</v>
@@ -1501,17 +1498,17 @@
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
       <c r="H8" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="8">
         <v>30</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -1522,16 +1519,16 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>61</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>62</v>
       </c>
       <c r="E9" s="28">
         <v>1</v>
@@ -1539,41 +1536,41 @@
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="8">
         <v>30</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="28">
         <v>1</v>
@@ -1581,11 +1578,11 @@
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="8">
         <v>30</v>
@@ -1593,7 +1590,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
@@ -1602,16 +1599,16 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="D11" s="27" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>32</v>
       </c>
       <c r="E11" s="28">
         <v>2</v>
@@ -1619,43 +1616,43 @@
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K11" s="8">
         <v>20</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="D12" s="27" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>37</v>
       </c>
       <c r="E12" s="28">
         <v>10</v>
@@ -1663,11 +1660,11 @@
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K12" s="8">
         <v>20</v>
@@ -1675,7 +1672,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -1684,16 +1681,16 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="D13" s="27" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>40</v>
       </c>
       <c r="E13" s="28">
         <v>10</v>
@@ -1701,11 +1698,11 @@
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="8">
         <v>20</v>
@@ -1713,7 +1710,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
@@ -1722,16 +1719,16 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="D14" s="27" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>43</v>
       </c>
       <c r="E14" s="28">
         <v>2</v>
@@ -1739,41 +1736,41 @@
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" s="8">
         <v>20</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="E15" s="28">
         <v>12</v>
@@ -1781,11 +1778,11 @@
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="30"/>
       <c r="J15" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" s="8">
         <v>20</v>
@@ -1793,7 +1790,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
@@ -1802,16 +1799,16 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="D16" s="27" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>48</v>
       </c>
       <c r="E16" s="28">
         <v>1</v>
@@ -1819,11 +1816,11 @@
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
       <c r="H16" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K16" s="8">
         <v>10</v>
@@ -1831,7 +1828,7 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
@@ -1840,16 +1837,16 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="D17" s="27" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>51</v>
       </c>
       <c r="E17" s="28">
         <v>1</v>
@@ -1857,41 +1854,41 @@
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K17" s="8">
         <v>10</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="D18" s="27" t="s">
         <v>53</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>54</v>
       </c>
       <c r="E18" s="28">
         <v>2</v>
@@ -1899,11 +1896,11 @@
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
       <c r="H18" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I18" s="30"/>
       <c r="J18" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K18" s="8">
         <v>30</v>
@@ -1911,7 +1908,7 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
@@ -1920,16 +1917,16 @@
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="28">
         <v>28</v>
@@ -1937,11 +1934,11 @@
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I19" s="30"/>
       <c r="J19" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K19" s="8">
         <v>30</v>
@@ -1949,7 +1946,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
@@ -1958,16 +1955,16 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="28">
         <v>14</v>
@@ -1975,11 +1972,11 @@
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I20" s="30"/>
       <c r="J20" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K20" s="8">
         <v>30</v>
@@ -1987,7 +1984,7 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
@@ -1996,16 +1993,16 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="D21" s="27" t="s">
         <v>67</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>68</v>
       </c>
       <c r="E21" s="28">
         <v>14</v>
@@ -2013,18 +2010,18 @@
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I21" s="30"/>
       <c r="J21" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K21" s="8">
         <v>20</v>
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
@@ -2034,16 +2031,16 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="D22" s="27" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>71</v>
       </c>
       <c r="E22" s="28">
         <v>84</v>
@@ -2051,11 +2048,11 @@
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I22" s="30"/>
       <c r="J22" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K22" s="8">
         <v>20</v>
@@ -2064,7 +2061,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
@@ -2072,16 +2069,16 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="D23" s="27" t="s">
         <v>73</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>74</v>
       </c>
       <c r="E23" s="28">
         <v>7</v>
@@ -2089,11 +2086,11 @@
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" s="8">
         <v>10</v>
@@ -2101,7 +2098,7 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
@@ -2110,16 +2107,16 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="27" t="s">
         <v>36</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>37</v>
       </c>
       <c r="E24" s="28">
         <v>42</v>
@@ -2127,39 +2124,39 @@
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I24" s="30"/>
       <c r="J24" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K24" s="8">
         <v>20</v>
       </c>
       <c r="L24" s="8"/>
       <c r="M24" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1">
       <c r="A25" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>44</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="E25" s="28">
         <v>84</v>
@@ -2167,11 +2164,11 @@
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I25" s="30"/>
       <c r="J25" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K25" s="8">
         <v>20</v>
@@ -2179,7 +2176,7 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
@@ -2193,7 +2190,7 @@
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
       <c r="F26" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="37">
         <f>SUM(G6:G25)</f>
@@ -2213,13 +2210,13 @@
     </row>
     <row r="30" spans="1:18">
       <c r="C30" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D30" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="39" t="s">
         <v>83</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -2227,10 +2224,10 @@
         <v>10</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:18">
@@ -2241,7 +2238,7 @@
         <v>11</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="3:5">
@@ -2252,101 +2249,101 @@
         <v>12</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="3:5">
       <c r="C34" s="39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="39" t="s">
         <v>86</v>
-      </c>
-      <c r="E34" s="39" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="35" spans="3:5">
       <c r="C35" s="39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="39" t="s">
         <v>99</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="3:5">
       <c r="C39" s="39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="3:5">
       <c r="C40" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="39" t="s">
         <v>88</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="41" spans="3:5">
       <c r="C41" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="3:5">
       <c r="C42" s="39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="3:5">
       <c r="C43" s="39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="3:5">
       <c r="C44" s="39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="3:5">
       <c r="C45" s="39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="3:5">
       <c r="C46" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="3:5">
       <c r="C47" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted fitBtn and Combobox.
</commit_message>
<xml_diff>
--- a/test_files/Przykładowy szablon.xlsx
+++ b/test_files/Przykładowy szablon.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$B$6:$R$6</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -324,9 +325,6 @@
     <t>Koniec</t>
   </si>
   <si>
-    <t>Wypalarka Sebastian</t>
-  </si>
-  <si>
     <t>St3</t>
   </si>
   <si>
@@ -345,7 +343,10 @@
     <t>S355</t>
   </si>
   <si>
-    <t>Gietarka Jacek</t>
+    <t>Wypalarka TEST</t>
+  </si>
+  <si>
+    <t>Gietarka TEST</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1382,7 +1383,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:19" ht="102" thickBot="1">
+    <row r="6" spans="1:19" ht="80.25" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>98</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>108</v>
@@ -1522,16 +1523,16 @@
         <v>28</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="28">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
@@ -1546,28 +1547,24 @@
         <v>30</v>
       </c>
       <c r="L9" s="8"/>
-      <c r="M9" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
-      <c r="Q9" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>61</v>
@@ -1578,7 +1575,7 @@
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="27" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="31" t="s">
@@ -1588,86 +1585,84 @@
         <v>30</v>
       </c>
       <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="M10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
+      <c r="Q10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E11" s="28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="27" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K11" s="8">
-        <v>20</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8" t="s">
         <v>55</v>
       </c>
       <c r="O11" s="8"/>
-      <c r="P11" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E12" s="28">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="27" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K12" s="8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
@@ -1684,21 +1679,21 @@
         <v>28</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E13" s="28">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="27" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="31" t="s">
@@ -1707,31 +1702,37 @@
       <c r="K13" s="8">
         <v>20</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8" t="s">
         <v>55</v>
       </c>
       <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="P13" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E14" s="28">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -1746,17 +1747,13 @@
         <v>20</v>
       </c>
       <c r="L14" s="8"/>
-      <c r="M14" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:19">
@@ -1764,16 +1761,16 @@
         <v>28</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E15" s="28">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
@@ -1788,13 +1785,15 @@
         <v>20</v>
       </c>
       <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="M15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="8"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="Q15" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="R15" s="8"/>
     </row>
     <row r="16" spans="1:19">
@@ -1802,28 +1801,28 @@
         <v>28</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E16" s="28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
       <c r="H16" s="27" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K16" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -1840,33 +1839,33 @@
         <v>28</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E17" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="27" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K17" s="8">
-        <v>10</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M17" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="N17" s="8"/>
       <c r="O17" s="8" t="s">
         <v>55</v>
@@ -1882,16 +1881,16 @@
         <v>28</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E18" s="28">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
@@ -1903,7 +1902,7 @@
         <v>33</v>
       </c>
       <c r="K18" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -1920,28 +1919,28 @@
         <v>28</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E19" s="28">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="27" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="I19" s="30"/>
       <c r="J19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K19" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1958,28 +1957,28 @@
         <v>28</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E20" s="28">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="27" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="I20" s="30"/>
       <c r="J20" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K20" s="8">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
@@ -1996,37 +1995,41 @@
         <v>28</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E21" s="28">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="27" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
       <c r="I21" s="30"/>
       <c r="J21" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K21" s="8">
-        <v>20</v>
-      </c>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="8"/>
       <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
+      <c r="O21" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
+      <c r="Q21" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="1:18">
@@ -2034,16 +2037,16 @@
         <v>28</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E22" s="28">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -2055,14 +2058,14 @@
         <v>33</v>
       </c>
       <c r="K22" s="8">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
+      <c r="M22" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="N22" s="8"/>
-      <c r="O22" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
@@ -2072,34 +2075,34 @@
         <v>28</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E23" s="28">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="27" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="I23" s="30"/>
       <c r="J23" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K23" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="M23" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" s="8"/>
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
@@ -2110,16 +2113,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E24" s="28">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
@@ -2134,15 +2137,13 @@
         <v>20</v>
       </c>
       <c r="L24" s="8"/>
-      <c r="M24" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="M24" s="8"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
+      <c r="O24" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="P24" s="8"/>
-      <c r="Q24" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="1:18" ht="15.75" thickBot="1">
@@ -2150,28 +2151,28 @@
         <v>28</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E25" s="28">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I25" s="30"/>
       <c r="J25" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K25" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -2347,6 +2348,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B6:R6">
+    <sortState ref="B7:R26">
+      <sortCondition ref="C6"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="5">
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="G2:I2"/>

</xml_diff>